<commit_message>
Se puede ingresar el nombre de la hoja y muestra un resumen
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcandiapereira/Documents/Desarrollo/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AF0DE4-7272-EB4F-BB48-23ED0758704F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A633BCB-402C-2D4C-A725-311EBA76B0B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,16 +18,17 @@
     <sheet name="16" sheetId="3" r:id="rId3"/>
     <sheet name="15" sheetId="4" r:id="rId4"/>
     <sheet name="14" sheetId="5" r:id="rId5"/>
-    <sheet name="13i" sheetId="6" r:id="rId6"/>
-    <sheet name="hoja" sheetId="7" r:id="rId7"/>
-    <sheet name="11" sheetId="8" r:id="rId8"/>
+    <sheet name="13" sheetId="6" r:id="rId6"/>
+    <sheet name="12" sheetId="7" r:id="rId7"/>
+    <sheet name="12b" sheetId="8" r:id="rId8"/>
+    <sheet name="11" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="205">
   <si>
     <t xml:space="preserve">AV VICUNA MACKENNA </t>
   </si>
@@ -419,13 +420,166 @@
     <t>LONGAVI </t>
   </si>
   <si>
+    <t>(2) 379-8533</t>
+  </si>
+  <si>
     <t>SANTA JULIA </t>
   </si>
   <si>
+    <t>(2) 282-9829</t>
+  </si>
+  <si>
+    <t>(2) 311-9025</t>
+  </si>
+  <si>
+    <t>(2) 315-8860</t>
+  </si>
+  <si>
+    <t>(2) 311-6625</t>
+  </si>
+  <si>
+    <t>(2) 454-1510</t>
+  </si>
+  <si>
+    <t>(2) 319-1535</t>
+  </si>
+  <si>
+    <t>(2) 281-6209</t>
+  </si>
+  <si>
+    <t>(2) 282-8702</t>
+  </si>
+  <si>
+    <t>(2) 291-1389</t>
+  </si>
+  <si>
+    <t>(2) 262-1652</t>
+  </si>
+  <si>
+    <t>(2) 282-4757</t>
+  </si>
+  <si>
+    <t>(2) 281-5055</t>
+  </si>
+  <si>
+    <t>(2) 262-0047</t>
+  </si>
+  <si>
+    <t>(2) 311-5034</t>
+  </si>
+  <si>
+    <t>(2) 493-7349</t>
+  </si>
+  <si>
+    <t>(2) 314-7502</t>
+  </si>
+  <si>
+    <t>(2) 314-3998</t>
+  </si>
+  <si>
+    <t>(2) 281-0493</t>
+  </si>
+  <si>
+    <t>(2) 313-5015</t>
+  </si>
+  <si>
+    <t>(2) 281-3435</t>
+  </si>
+  <si>
+    <t>(2) 769-3710</t>
+  </si>
+  <si>
+    <t>(2) 282-0509</t>
+  </si>
+  <si>
     <t>ANIBAL PINTO</t>
   </si>
   <si>
+    <t>(2) 282-2190</t>
+  </si>
+  <si>
+    <t>(2) 291-7855</t>
+  </si>
+  <si>
+    <t>(2) 313-1457</t>
+  </si>
+  <si>
+    <t>(2) 329-0223</t>
+  </si>
+  <si>
+    <t>(2) 281-0831</t>
+  </si>
+  <si>
+    <t>(2) 282-7668</t>
+  </si>
+  <si>
+    <t>(2) 281-2058</t>
+  </si>
+  <si>
+    <t>(2) 315-7002</t>
+  </si>
+  <si>
+    <t>(2) 314-8715</t>
+  </si>
+  <si>
+    <t>(2) 281-8873</t>
+  </si>
+  <si>
+    <t>(2) 262-5681</t>
+  </si>
+  <si>
+    <t>(2) 311-9961</t>
+  </si>
+  <si>
+    <t>(2) 319-8092</t>
+  </si>
+  <si>
+    <t>(2) 315-4161</t>
+  </si>
+  <si>
+    <t>(2) 493-1635</t>
+  </si>
+  <si>
+    <t>(2) 262-2966</t>
+  </si>
+  <si>
+    <t>(2) 281-2183</t>
+  </si>
+  <si>
     <t>PADRE HURTADO</t>
+  </si>
+  <si>
+    <t>(2) 725-5585</t>
+  </si>
+  <si>
+    <t>(2) 417-6876</t>
+  </si>
+  <si>
+    <t>(2) 313-4602</t>
+  </si>
+  <si>
+    <t>(2) 313-4823</t>
+  </si>
+  <si>
+    <t>(2) 282-7751</t>
+  </si>
+  <si>
+    <t>(2) 262-7451</t>
+  </si>
+  <si>
+    <t>(2) 311-8012</t>
+  </si>
+  <si>
+    <t>(2) 262-7142</t>
+  </si>
+  <si>
+    <t>(2) 291-7967</t>
+  </si>
+  <si>
+    <t>(2) 493-2039</t>
+  </si>
+  <si>
+    <t>(2) 281-7679</t>
   </si>
   <si>
     <t>MONSENOR LIZAMA</t>
@@ -9973,10 +10127,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B188"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9984,1508 +10138,1049 @@
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>8473</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>8445</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>8461</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4">
         <v>8469</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5">
         <v>8585</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B6">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B9">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B12">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B14">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B15">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B17">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B18">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B19">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B20">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B21">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B22">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B24">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B25">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B26">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B27">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B28">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B29">
         <v>133</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B30">
         <v>141</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B31">
         <v>157</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B32">
         <v>165</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B33">
         <v>173</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B34">
         <v>179</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>181</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>189</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37">
         <v>193</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B38">
         <v>207</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B39">
         <v>229</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B40">
         <v>249</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B41">
         <v>251</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B42">
         <v>261</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B43">
         <v>267</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B44">
         <v>275</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B45">
         <v>283</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B46">
         <v>291</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B47">
         <v>299</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B48">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B49">
         <v>33</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B50">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B51">
         <v>45</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B53">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B54">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B55">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B56">
         <v>81</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B57">
         <v>87</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B58">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B59">
         <v>30</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B60">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B61">
         <v>46</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B62">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B63">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B64">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B65">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B66">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B67">
         <v>86</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B68">
         <v>88</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B69">
         <v>8463</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B70">
         <v>8455</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B71">
         <v>8447</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B72">
         <v>8439</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B73">
         <v>8431</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B74">
         <v>8466</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B75">
         <v>8454</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B76">
         <v>8446</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B77">
         <v>8434</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B78">
         <v>8422</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B79">
         <v>8410</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B80">
         <v>8478</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B81">
         <v>8411</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B82">
         <v>8423</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B83">
         <v>8435</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B84">
         <v>8447</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B85">
         <v>8453</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="B86">
         <v>8467</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B87">
         <v>204</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B88">
         <v>208</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B89">
         <v>212</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B90">
         <v>216</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B91">
         <v>220</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B92">
         <v>224</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B93">
         <v>228</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B94">
         <v>232</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="B95">
         <v>236</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B96">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B97">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B98">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B99">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B100">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B101">
-        <v>8414</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B102">
-        <v>8426</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B103">
-        <v>8438</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B104">
-        <v>8448</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B105">
-        <v>8452</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B106">
-        <v>8468</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B107">
-        <v>8415</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B108">
-        <v>8427</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B109">
-        <v>8439</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B110">
-        <v>8443</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B111">
-        <v>8451</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B112">
-        <v>8469</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B113">
-        <v>8479</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B114">
-        <v>8481</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B115">
-        <v>8489</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B116">
-        <v>8412</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B117">
-        <v>8424</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B118">
-        <v>8436</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B119">
-        <v>8448</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B120">
-        <v>8413</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121">
-        <v>8425</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B122">
-        <v>8437</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B123">
-        <v>8449</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B124">
-        <v>8470</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B125">
-        <v>8482</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B126">
-        <v>8496</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B127">
-        <v>8508</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B128">
-        <v>8514</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B129">
-        <v>8522</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B130">
-        <v>8536</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B131">
-        <v>8548</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B132">
-        <v>8554</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B133">
-        <v>8566</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B134">
-        <v>8568</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B135">
-        <v>8574</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B136">
-        <v>8588</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B137">
-        <v>8537</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B138">
-        <v>8549</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B139">
-        <v>8555</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B140">
-        <v>8573</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B141">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B142">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B143">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B144">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B145">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B146">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B147">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B148">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B149">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B150">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B151">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B152">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B153">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B154">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B155">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B156">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B157">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B158">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B159">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B160">
-        <v>8584</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B161">
-        <v>8572</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B162">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B163">
-        <v>8571</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B164">
-        <v>8583</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B165">
-        <v>8589</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B166">
-        <v>8588</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B167">
-        <v>8580</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B168">
-        <v>8574</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B169">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B170">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B171">
-        <v>8575</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B172">
-        <v>8581</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B173">
-        <v>8589</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B174">
-        <v>8586</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B175">
-        <v>8570</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B176">
-        <v>8574</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B177">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B178">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B179">
-        <v>8577</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B180">
-        <v>8581</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B181">
-        <v>8587</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B182">
-        <v>8592</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B183">
-        <v>8582</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B184">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B185">
-        <v>8573</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B186">
-        <v>8581</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B187">
-        <v>8587</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B188">
-        <v>8591</v>
+      <c r="C95" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -11496,9 +11191,768 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection sqref="A1:B93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6">
+        <v>8414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7">
+        <v>8426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8">
+        <v>8438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9">
+        <v>8448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10">
+        <v>8452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11">
+        <v>8468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12">
+        <v>8415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13">
+        <v>8427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14">
+        <v>8439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15">
+        <v>8443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16">
+        <v>8451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17">
+        <v>8469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18">
+        <v>8479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19">
+        <v>8481</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20">
+        <v>8489</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21">
+        <v>8412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22">
+        <v>8424</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23">
+        <v>8436</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24">
+        <v>8448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25">
+        <v>8413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26">
+        <v>8425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27">
+        <v>8437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28">
+        <v>8449</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29">
+        <v>8470</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30">
+        <v>8482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31">
+        <v>8496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32">
+        <v>8508</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34">
+        <v>8522</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35">
+        <v>8536</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36">
+        <v>8548</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37">
+        <v>8554</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38">
+        <v>8566</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39">
+        <v>8568</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40">
+        <v>8574</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41">
+        <v>8588</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42">
+        <v>8537</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43">
+        <v>8549</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44">
+        <v>8555</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45">
+        <v>8573</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B47">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B61">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65">
+        <v>8584</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B66">
+        <v>8572</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68">
+        <v>8571</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69">
+        <v>8583</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B71">
+        <v>8588</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73">
+        <v>8574</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76">
+        <v>8575</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B78">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79">
+        <v>8586</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B80">
+        <v>8570</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B81">
+        <v>8574</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B83">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B84">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87">
+        <v>8592</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B88">
+        <v>8582</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B89">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B90">
+        <v>8573</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B91">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B92">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B93">
+        <v>8591</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView zoomScale="181" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -11506,7 +11960,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B1">
         <v>568</v>
@@ -11517,7 +11971,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>567</v>
@@ -11528,18 +11982,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B3">
         <v>584</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B4">
         <v>592</v>
@@ -11550,18 +12004,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B5">
         <v>618</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>626</v>
@@ -11572,18 +12026,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B7">
         <v>634</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B8">
         <v>642</v>
@@ -11594,7 +12048,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B9">
         <v>664</v>
@@ -11605,7 +12059,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B10">
         <v>676</v>
@@ -11616,18 +12070,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B11">
         <v>688</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B12">
         <v>696</v>
@@ -11638,18 +12092,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B13">
         <v>746</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B14">
         <v>754</v>
@@ -11660,7 +12114,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B15">
         <v>758</v>
@@ -11671,29 +12125,29 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B16">
         <v>764</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B17">
         <v>774</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B18">
         <v>782</v>
@@ -11704,51 +12158,51 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B19">
         <v>832</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B20">
         <v>844</v>
       </c>
       <c r="C20" t="s">
-        <v>151</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B21">
         <v>852</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B22">
         <v>864</v>
       </c>
       <c r="C22" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B23">
         <v>876</v>
@@ -11759,7 +12213,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="B24">
         <v>888</v>

</xml_diff>